<commit_message>
Update for new layout
</commit_message>
<xml_diff>
--- a/Garage-Layout/EX-CommandStation/Pin Alias Workings.xlsx
+++ b/Garage-Layout/EX-CommandStation/Pin Alias Workings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\DCC-EX-configs\Garage-Layout\EX-CommandStation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC043F6-C592-48DE-B066-7676369A68AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E509F08B-8D41-417F-A6F5-2DB0AECA0CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{09D121E1-19B1-4886-9784-2A472DF88890}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>_DIR</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>RESET(POINT_POWER)</t>
+  </si>
+  <si>
+    <t>Macro</t>
+  </si>
+  <si>
+    <t>ROKUHANPOINT(</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFE0C65-0EB3-477D-8D75-9206151FCA59}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,9 +470,10 @@
     <col min="10" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -503,8 +510,11 @@
       <c r="L1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -549,8 +559,12 @@
         <f>CONCATENATE($A$9,$F2,$A$6)</f>
         <v>RESET(POINT1_EN)</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" t="str">
+        <f>CONCATENATE($A$10,B2,$A$5,E2,$A$5,F2,$A$5,"",$A$5,"POINT",B2,$A$6)</f>
+        <v>ROKUHANPOINT(1,POINT1_DIR,POINT1_EN,,POINT1)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -572,11 +586,11 @@
         <v>POINT2_EN</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G23" si="2">CONCATENATE($A$1,E3,$A$5,C3,$A$6)</f>
+        <f t="shared" ref="G3:G22" si="2">CONCATENATE($A$1,E3,$A$5,C3,$A$6)</f>
         <v>ALIAS(POINT2_DIR,165)</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H23" si="3">CONCATENATE($A$1,F3,$A$5,D3,$A$6)</f>
+        <f t="shared" ref="H3:H22" si="3">CONCATENATE($A$1,F3,$A$5,D3,$A$6)</f>
         <v>ALIAS(POINT2_EN,173)</v>
       </c>
       <c r="I3" t="str">
@@ -595,8 +609,12 @@
         <f t="shared" ref="L3:L23" si="7">CONCATENATE($A$9,$F3,$A$6)</f>
         <v>RESET(POINT2_EN)</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M22" si="8">CONCATENATE($A$10,B3,$A$5,E3,$A$5,F3,$A$5,"",$A$5,"POINT",B3,$A$6)</f>
+        <v>ROKUHANPOINT(2,POINT2_DIR,POINT2_EN,,POINT2)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -641,8 +659,12 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT3_EN)</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(3,POINT3_DIR,POINT3_EN,,POINT3)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -687,8 +709,12 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT4_EN)</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(4,POINT4_DIR,POINT4_EN,,POINT4)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -733,8 +759,12 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT5_EN)</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(5,POINT5_DIR,POINT5_EN,,POINT5)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>6</v>
       </c>
@@ -776,8 +806,12 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT6_EN)</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(6,POINT6_DIR,POINT6_EN,,POINT6)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -822,8 +856,12 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT7_EN)</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(7,POINT7_DIR,POINT7_EN,,POINT7)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -868,16 +906,23 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT8_EN)</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(8,POINT8_DIR,POINT8_EN,,POINT8)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D10">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -889,11 +934,11 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT9_DIR,179)</v>
+        <v>ALIAS(POINT9_DIR,180)</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT9_EN,187)</v>
+        <v>ALIAS(POINT9_EN,188)</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="4"/>
@@ -911,16 +956,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT9_EN)</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(9,POINT9_DIR,POINT9_EN,,POINT9)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D11">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -932,11 +981,11 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT10_DIR,180)</v>
+        <v>ALIAS(POINT10_DIR,181)</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT10_EN,188)</v>
+        <v>ALIAS(POINT10_EN,189)</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="4"/>
@@ -954,16 +1003,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT10_EN)</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(10,POINT10_DIR,POINT10_EN,,POINT10)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D12">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -975,11 +1028,11 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT11_DIR,181)</v>
+        <v>ALIAS(POINT11_DIR,182)</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT11_EN,189)</v>
+        <v>ALIAS(POINT11_EN,190)</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="4"/>
@@ -997,16 +1050,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT11_EN)</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(11,POINT11_DIR,POINT11_EN,,POINT11)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D13">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -1018,11 +1075,11 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT12_DIR,182)</v>
+        <v>ALIAS(POINT12_DIR,183)</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT12_EN,190)</v>
+        <v>ALIAS(POINT12_EN,191)</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="4"/>
@@ -1040,16 +1097,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT12_EN)</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(12,POINT12_DIR,POINT12_EN,,POINT12)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D14">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -1061,11 +1122,11 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT13_DIR,183)</v>
+        <v>ALIAS(POINT13_DIR,184)</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT13_EN,191)</v>
+        <v>ALIAS(POINT13_EN,192)</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="4"/>
@@ -1083,16 +1144,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT13_EN)</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(13,POINT13_DIR,POINT13_EN,,POINT13)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D15">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -1104,11 +1169,11 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT14_DIR,184)</v>
+        <v>ALIAS(POINT14_DIR,185)</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT14_EN,192)</v>
+        <v>ALIAS(POINT14_EN,193)</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="4"/>
@@ -1126,16 +1191,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT14_EN)</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(14,POINT14_DIR,POINT14_EN,,POINT14)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D16">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -1147,11 +1216,11 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT15_DIR,185)</v>
+        <v>ALIAS(POINT15_DIR,186)</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT15_EN,193)</v>
+        <v>ALIAS(POINT15_EN,194)</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="4"/>
@@ -1169,16 +1238,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT15_EN)</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M16" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(15,POINT15_DIR,POINT15_EN,,POINT15)</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D17">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -1190,11 +1263,11 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT16_DIR,186)</v>
+        <v>ALIAS(POINT16_DIR,187)</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT16_EN,194)</v>
+        <v>ALIAS(POINT16_EN,195)</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="4"/>
@@ -1212,16 +1285,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT16_EN)</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M17" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(16,POINT16_DIR,POINT16_EN,,POINT16)</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="D18">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -1233,11 +1310,11 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT17_DIR,187)</v>
+        <v>ALIAS(POINT17_DIR,196)</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT17_EN,195)</v>
+        <v>ALIAS(POINT17_EN,204)</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="4"/>
@@ -1255,16 +1332,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT17_EN)</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M18" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(17,POINT17_DIR,POINT17_EN,,POINT17)</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D19">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -1276,11 +1357,11 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT18_DIR,196)</v>
+        <v>ALIAS(POINT18_DIR,197)</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT18_EN,204)</v>
+        <v>ALIAS(POINT18_EN,205)</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="4"/>
@@ -1298,16 +1379,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT18_EN)</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M19" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(18,POINT18_DIR,POINT18_EN,,POINT18)</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D20">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -1319,11 +1404,11 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT19_DIR,197)</v>
+        <v>ALIAS(POINT19_DIR,198)</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT19_EN,205)</v>
+        <v>ALIAS(POINT19_EN,206)</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="4"/>
@@ -1341,16 +1426,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT19_EN)</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M20" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(19,POINT19_DIR,POINT19_EN,,POINT19)</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D21">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -1362,11 +1451,11 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT20_DIR,198)</v>
+        <v>ALIAS(POINT20_DIR,199)</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT20_EN,206)</v>
+        <v>ALIAS(POINT20_EN,207)</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="4"/>
@@ -1384,16 +1473,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT20_EN)</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M21" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(20,POINT20_DIR,POINT20_EN,,POINT20)</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D22">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
@@ -1405,11 +1498,11 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="2"/>
-        <v>ALIAS(POINT21_DIR,199)</v>
+        <v>ALIAS(POINT21_DIR,200)</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="3"/>
-        <v>ALIAS(POINT21_EN,207)</v>
+        <v>ALIAS(POINT21_EN,208)</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="4"/>
@@ -1427,16 +1520,20 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT21_EN)</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M22" t="str">
+        <f t="shared" si="8"/>
+        <v>ROKUHANPOINT(21,POINT21_DIR,POINT21_EN,,POINT21)</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D23">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -1447,12 +1544,12 @@
         <v>POINT22_EN</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="2"/>
-        <v>ALIAS(POINT22_DIR,200)</v>
+        <f t="shared" ref="G23" si="9">CONCATENATE($A$1,E23,$A$5,C23,$A$6)</f>
+        <v>ALIAS(POINT22_DIR,201)</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="3"/>
-        <v>ALIAS(POINT22_EN,208)</v>
+        <f t="shared" ref="H23" si="10">CONCATENATE($A$1,F23,$A$5,D23,$A$6)</f>
+        <v>ALIAS(POINT22_EN,209)</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="4"/>
@@ -1470,49 +1567,36 @@
         <f t="shared" si="7"/>
         <v>RESET(POINT22_EN)</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>23</v>
-      </c>
+      <c r="M23" t="str">
+        <f t="shared" ref="M23" si="11">CONCATENATE($A$10,B23,$A$5,E23,$A$5,F23,$A$5,"",$A$5,"POINT",B23,$A$6)</f>
+        <v>ROKUHANPOINT(22,POINT22_DIR,POINT22_EN,,POINT22)</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C24">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D24">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>24</v>
-      </c>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C25">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D25">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>25</v>
-      </c>
-      <c r="C26">
-        <v>203</v>
-      </c>
-      <c r="D26">
         <v>211</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F25" t="s">
         <v>16</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G25" t="s">
         <v>4</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I25" t="s">
         <v>21</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J25" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>